<commit_message>
Built case review spreadsheet for Kristen
</commit_message>
<xml_diff>
--- a/examples/UCH North Q4 2019.xlsx
+++ b/examples/UCH North Q4 2019.xlsx
@@ -8072,8 +8072,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010055E7AF632A704D4CBB1BD9FA14B19970" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="787e44dd84078b6165072bff64e09332">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="edae88a8-d9dc-4074-a55b-fb97cb2cd74d" xmlns:ns3="852f286e-3e14-48be-b416-81218d12f978" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2d4e4cd38ab3a23f51fecc8c992a902" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010055E7AF632A704D4CBB1BD9FA14B19970" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c915b622f17d06218f3334f54ec812be">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="edae88a8-d9dc-4074-a55b-fb97cb2cd74d" xmlns:ns3="852f286e-3e14-48be-b416-81218d12f978" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a3db0db921c34a782b6d64d961a8785" ns1:_="" ns2:_="" ns3:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="edae88a8-d9dc-4074-a55b-fb97cb2cd74d"/>
     <xsd:import namespace="852f286e-3e14-48be-b416-81218d12f978"/>
     <xsd:element name="properties">
@@ -8093,11 +8094,28 @@
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="20" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="21" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="edae88a8-d9dc-4074-a55b-fb97cb2cd74d" elementFormDefault="qualified">
@@ -8150,6 +8168,11 @@
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -8284,7 +8307,10 @@
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
 </p:properties>
 </file>
 
@@ -8298,22 +8324,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C11F35B9-4DBD-496F-9902-DDAD3F63A33C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="edae88a8-d9dc-4074-a55b-fb97cb2cd74d"/>
-    <ds:schemaRef ds:uri="852f286e-3e14-48be-b416-81218d12f978"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF17D625-A8A5-4B3E-B27E-D640CC166C5C}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Reinstalled insync on Linux and pulled 2022 Q4 data
</commit_message>
<xml_diff>
--- a/examples/UCH North Q4 2019.xlsx
+++ b/examples/UCH North Q4 2019.xlsx
@@ -8072,8 +8072,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010055E7AF632A704D4CBB1BD9FA14B19970" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c915b622f17d06218f3334f54ec812be">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="edae88a8-d9dc-4074-a55b-fb97cb2cd74d" xmlns:ns3="852f286e-3e14-48be-b416-81218d12f978" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a3db0db921c34a782b6d64d961a8785" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010055E7AF632A704D4CBB1BD9FA14B19970" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5705bc62546c00eb30d3e393ea3d800">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="edae88a8-d9dc-4074-a55b-fb97cb2cd74d" xmlns:ns3="852f286e-3e14-48be-b416-81218d12f978" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c29e53287aa3a112937d5a643cee4298" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="edae88a8-d9dc-4074-a55b-fb97cb2cd74d"/>
     <xsd:import namespace="852f286e-3e14-48be-b416-81218d12f978"/>
@@ -8097,6 +8097,8 @@
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -8175,6 +8177,13 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="23" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c6d7f816-bc26-4675-b66e-019c6d6df9c2" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="852f286e-3e14-48be-b416-81218d12f978" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -8204,6 +8213,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="24" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{470e1751-435f-4e7f-a343-fe3c661a44ef}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="852f286e-3e14-48be-b416-81218d12f978">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -8310,6 +8330,10 @@
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="852f286e-3e14-48be-b416-81218d12f978" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="edae88a8-d9dc-4074-a55b-fb97cb2cd74d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
 </file>
@@ -8324,7 +8348,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF17D625-A8A5-4B3E-B27E-D640CC166C5C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8357B4A8-0B2C-483D-A3AA-013BE5D58AC8}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>